<commit_message>
ADD results from server
</commit_message>
<xml_diff>
--- a/results/[10_hot_summers]_#_co2_price.xlsx
+++ b/results/[10_hot_summers]_#_co2_price.xlsx
@@ -447,7 +447,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>210</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -478,7 +478,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>230</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +540,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>270</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -571,7 +571,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>290</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>308</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>